<commit_message>
tweaked how to grab/display tools, parts and materials.
</commit_message>
<xml_diff>
--- a/templates/TRG MTA Template alt.xlsx
+++ b/templates/TRG MTA Template alt.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicho\OneDrive\Desktop\Dev Projects\MTA-Converter\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A155769-5E60-4A34-ACBA-FCB6427C80B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CC33528-17C1-4488-9D21-2D6BAAD5DF04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="7755" windowWidth="29040" windowHeight="15840" xr2:uid="{BD0F5AF9-A1D1-4FF0-999C-B0E32531BFC3}"/>
+    <workbookView minimized="1" xWindow="57600" yWindow="11160" windowWidth="9600" windowHeight="4605" xr2:uid="{BD0F5AF9-A1D1-4FF0-999C-B0E32531BFC3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2720,8 +2720,7 @@
 Stepladder</t>
   </si>
   <si>
-    <t>ADAPTER CAM &amp; GROOVE, TYPE F, BRASS 1-1/2" C&amp;G X 1-1/2" MPT MATERIAL AND DIMENSIONS IAW A-A-59326
-ADAPTER, CAM &amp; GROOVE, TYPE F Hard Coat Aluminum, 2" C&amp;G, x 2" MPT, material &amp; dimensions iaw A-A-59326</t>
+    <t>fAN, AIR EXHUAST, 8.86" x 8.86" x 3.15" 606 CFM @ 0, 115C, 50/60HZ</t>
   </si>
 </sst>
 </file>
@@ -4177,9 +4176,9 @@
   <dimension ref="A1:T337"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A119" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="2" topLeftCell="A113" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
-      <selection pane="bottomLeft" activeCell="J97" sqref="J97"/>
+      <selection pane="bottomLeft" activeCell="J115" sqref="J115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -9932,7 +9931,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="97" spans="1:20" ht="174" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:20" ht="145" x14ac:dyDescent="0.35">
       <c r="A97" s="19" t="s">
         <v>198</v>
       </c>

</xml_diff>